<commit_message>
Update sample closure Excel files (BU A/B/C 2025-02)
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/samples/closure_excel/closure_bu_a_202502.xlsx
+++ b/samples/closure_excel/closure_bu_a_202502.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,6 +555,66 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>40500</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BRL</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ACC-BU_A-0004</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Sample closure line 4 for BU_A</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2025-02-15</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>BU_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>50500</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>BRL</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ACC-BU_A-0005</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Sample closure line 5 for BU_A</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2025-02-15</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>BU_A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>